<commit_message>
This is a commit that combined the two commits with working guages
When I got the RPM and Input Voltage guages working, I had some trouble
committing the changes. I had one commit with all my object/junk files,
and another commit without the object/junk files (and some minor changes
to source code). To fix this, I decided to squash the commits together
into one "combination" commit. All files are up to date.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="67">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -198,6 +198,24 @@
   </si>
   <si>
     <t xml:space="preserve">Input Voltage: &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Typography_01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Timer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RPM: &lt;value&gt; rpm(s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Input Voltage: &lt;value&gt; V</t>
   </si>
 </sst>
 </file>
@@ -1478,10 +1496,10 @@
         <v>17</v>
       </c>
       <c r="G5"/>
-      <c r="H5" t="s">
-        <v>53</v>
-      </c>
-      <c r="I5"/>
+      <c r="H5"/>
+      <c r="I5" t="s">
+        <v>42</v>
+      </c>
       <c r="J5"/>
       <c r="L5" s="7" t="s">
         <v>1</v>
@@ -1515,7 +1533,9 @@
       </c>
       <c r="G6"/>
       <c r="H6"/>
-      <c r="I6"/>
+      <c r="I6" t="s">
+        <v>42</v>
+      </c>
       <c r="J6"/>
       <c r="L6" s="7" t="s">
         <v>2</v>
@@ -1549,7 +1569,9 @@
       </c>
       <c r="G7"/>
       <c r="H7"/>
-      <c r="I7"/>
+      <c r="I7" t="s">
+        <v>42</v>
+      </c>
       <c r="J7"/>
       <c r="L7" s="7" t="s">
         <v>7</v>
@@ -1568,6 +1590,27 @@
       </c>
     </row>
     <row r="8" spans="2:16">
+      <c r="B8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8">
+        <v>26</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="I8" t="s">
+        <v>42</v>
+      </c>
+      <c r="J8"/>
       <c r="L8" s="7" t="s">
         <v>8</v>
       </c>
@@ -1712,7 +1755,7 @@
         <v>45</v>
       </c>
       <c r="F5" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6">
@@ -1729,7 +1772,7 @@
         <v>45</v>
       </c>
       <c r="F6" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7">
@@ -1737,7 +1780,7 @@
         <v>54</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="D7" t="s">
         <v>49</v>
@@ -1746,10 +1789,26 @@
         <v>45</v>
       </c>
       <c r="F7" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
     </row>
-    <row r="8"/>
+    <row r="8">
+      <c r="B8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" t="s">
+        <v>64</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Restructured and Organized Timer Guage
Timer guage reorganized nice and neatly, numbers increment and are
showing. InVolt and RPM guages still not resetting back to default
values, but CAN line messages update them when received.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="67">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1800,13 +1800,13 @@
         <v>61</v>
       </c>
       <c r="D8" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="E8" t="s">
         <v>45</v>
       </c>
       <c r="F8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>